<commit_message>
Update BPF Winding Data
Update BPF Winding Data
</commit_message>
<xml_diff>
--- a/T41_V012_Files_01-15-24/T41_V012_BOMs/T41_Main_Board_BOM_All_V12.6_12-26-23.xlsx
+++ b/T41_V012_Files_01-15-24/T41_V012_BOMs/T41_Main_Board_BOM_All_V12.6_12-26-23.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dad\Documents\T41\V012 Files\BOMs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dad\Documents\GitHub\T41\T41_V012_Files_01-15-24\T41_V012_BOMs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0174FD16-60FC-4323-9932-A2E6FA7B20AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B167179-00D5-4D9B-82AF-74BB89852B81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Board Summary" sheetId="6" r:id="rId1"/>
@@ -112,9 +112,6 @@
   </si>
   <si>
     <t>Q1</t>
-  </si>
-  <si>
-    <t>942-IRF4905PBF</t>
   </si>
   <si>
     <t>100 Ohm SMD 1206 Resistor</t>
@@ -562,9 +559,6 @@
   </si>
   <si>
     <t>LM1117T-3.3 LDO Voltage Reg. TO-220-3</t>
-  </si>
-  <si>
-    <t>IRF4095PBF MOSFET 70A TO-220-3</t>
   </si>
   <si>
     <t>2N7000 TO-92</t>
@@ -793,6 +787,12 @@
       </rPr>
       <t xml:space="preserve"> but NOT BOTH</t>
     </r>
+  </si>
+  <si>
+    <t>SUP90P06-09L-E3 MOSFET 90A TO-220-3</t>
+  </si>
+  <si>
+    <t>781-SUP90P06-09L-E3</t>
   </si>
 </sst>
 </file>
@@ -1561,9 +1561,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1601,7 +1601,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1707,7 +1707,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1849,7 +1849,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1863,46 +1863,46 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.36328125" customWidth="1"/>
-    <col min="2" max="2" width="24.90625" customWidth="1"/>
-    <col min="4" max="4" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.33203125" customWidth="1"/>
+    <col min="2" max="2" width="24.88671875" customWidth="1"/>
+    <col min="4" max="4" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="26" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:11" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="18" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="26" x14ac:dyDescent="0.6">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A2" s="18"/>
     </row>
-    <row r="3" spans="1:11" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="19" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C3" s="20"/>
       <c r="D3" s="19" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E3" s="19" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="21">
+        <v>1</v>
+      </c>
+      <c r="B5" s="22" t="s">
         <v>166</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="21">
-        <v>1</v>
-      </c>
-      <c r="B5" s="22" t="s">
-        <v>168</v>
       </c>
       <c r="C5" s="22"/>
       <c r="D5" s="21">
@@ -1911,7 +1911,7 @@
       </c>
       <c r="E5" s="23">
         <f>'Base Board'!I44</f>
-        <v>89.441999999999979</v>
+        <v>92.221999999999994</v>
       </c>
       <c r="F5" s="22"/>
       <c r="G5" s="22"/>
@@ -1920,12 +1920,12 @@
       <c r="J5" s="22"/>
       <c r="K5" s="22"/>
     </row>
-    <row r="6" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="21">
         <v>5</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C6" s="22"/>
       <c r="D6" s="21">
@@ -1943,12 +1943,12 @@
       <c r="J6" s="22"/>
       <c r="K6" s="22"/>
     </row>
-    <row r="7" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="21">
         <v>6</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C7" s="22"/>
       <c r="D7" s="21">
@@ -1966,7 +1966,7 @@
       <c r="J7" s="22"/>
       <c r="K7" s="22"/>
     </row>
-    <row r="8" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="22"/>
       <c r="B8" s="22"/>
       <c r="C8" s="22"/>
@@ -1976,7 +1976,7 @@
       </c>
       <c r="E8" s="26">
         <f>SUM(E5:E7)</f>
-        <v>93.749999999999972</v>
+        <v>96.529999999999987</v>
       </c>
       <c r="F8" s="22"/>
       <c r="G8" s="22"/>
@@ -1985,7 +1985,7 @@
       <c r="J8" s="22"/>
       <c r="K8" s="22"/>
     </row>
-    <row r="9" spans="1:11" ht="16" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A9" s="22"/>
       <c r="B9" s="22"/>
       <c r="C9" s="22"/>
@@ -1998,7 +1998,7 @@
       <c r="J9" s="22"/>
       <c r="K9" s="22"/>
     </row>
-    <row r="10" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="22"/>
       <c r="B10" s="22"/>
       <c r="C10" s="22"/>
@@ -2011,10 +2011,10 @@
       <c r="J10" s="22"/>
       <c r="K10" s="22"/>
     </row>
-    <row r="11" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="22"/>
       <c r="B11" s="27" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C11" s="22"/>
       <c r="D11" s="22"/>
@@ -2026,7 +2026,7 @@
       <c r="J11" s="22"/>
       <c r="K11" s="22"/>
     </row>
-    <row r="12" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="22"/>
       <c r="B12" s="22"/>
       <c r="C12" s="22"/>
@@ -2052,25 +2052,25 @@
   </sheetPr>
   <dimension ref="A1:J56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.55" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8" style="8" customWidth="1"/>
-    <col min="2" max="2" width="36.36328125" customWidth="1"/>
-    <col min="3" max="3" width="59.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.54296875" customWidth="1"/>
-    <col min="5" max="5" width="21.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.26953125" customWidth="1"/>
-    <col min="7" max="7" width="14.81640625" customWidth="1"/>
-    <col min="8" max="8" width="11.36328125" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.33203125" customWidth="1"/>
+    <col min="3" max="3" width="59.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.5546875" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.21875" customWidth="1"/>
+    <col min="7" max="7" width="14.77734375" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -2087,22 +2087,22 @@
         <v>4</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
         <v>15</v>
       </c>
@@ -2110,7 +2110,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -2123,18 +2123,18 @@
         <v>0.80999999999999994</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" t="s">
         <v>74</v>
-      </c>
-      <c r="D3" t="s">
-        <v>75</v>
       </c>
       <c r="H3" s="13">
         <v>0.1</v>
@@ -2144,7 +2144,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <v>1</v>
       </c>
@@ -2165,7 +2165,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>2</v>
       </c>
@@ -2173,13 +2173,13 @@
         <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D5" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="H5" s="13">
         <v>0.17</v>
@@ -2189,7 +2189,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <v>11</v>
       </c>
@@ -2197,10 +2197,10 @@
         <v>11</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H6" s="10">
         <v>0.28999999999999998</v>
@@ -2210,7 +2210,7 @@
         <v>3.19</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>3</v>
       </c>
@@ -2231,7 +2231,7 @@
         <v>1.17</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <v>1</v>
       </c>
@@ -2242,7 +2242,7 @@
         <v>16</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H8" s="13">
         <v>0.24</v>
@@ -2252,7 +2252,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <v>3</v>
       </c>
@@ -2263,7 +2263,7 @@
         <v>18</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>20</v>
@@ -2276,18 +2276,18 @@
         <v>0.84000000000000008</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
         <v>1</v>
       </c>
       <c r="B10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C10" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="C10" s="30" t="s">
+      <c r="D10" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>109</v>
       </c>
       <c r="E10" s="1"/>
       <c r="H10" s="13">
@@ -2298,7 +2298,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <v>4</v>
       </c>
@@ -2306,16 +2306,16 @@
         <v>19</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>20</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H11" s="13">
         <v>1.41</v>
@@ -2325,7 +2325,7 @@
         <v>5.64</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8">
         <v>3</v>
       </c>
@@ -2336,7 +2336,7 @@
         <v>22</v>
       </c>
       <c r="D12" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E12" t="s">
         <v>20</v>
@@ -2349,42 +2349,42 @@
         <v>1.41</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8">
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>141</v>
+        <v>175</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D13" t="s">
-        <v>24</v>
+        <v>176</v>
       </c>
       <c r="E13" t="s">
         <v>20</v>
       </c>
       <c r="H13" s="13">
-        <v>2.27</v>
+        <v>5.05</v>
       </c>
       <c r="I13" s="14">
         <f t="shared" si="0"/>
-        <v>2.27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>5.05</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8">
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H14" s="13">
         <v>0.36</v>
@@ -2394,18 +2394,18 @@
         <v>0.72</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8">
         <v>3</v>
       </c>
       <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" t="s">
         <v>26</v>
-      </c>
-      <c r="D15" t="s">
-        <v>27</v>
       </c>
       <c r="H15" s="13">
         <v>0.1</v>
@@ -2415,18 +2415,18 @@
         <v>0.30000000000000004</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8">
         <v>1</v>
       </c>
       <c r="B16" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" t="s">
         <v>78</v>
-      </c>
-      <c r="D16" t="s">
-        <v>79</v>
       </c>
       <c r="H16" s="13">
         <v>0.1</v>
@@ -2436,18 +2436,18 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8">
         <v>2</v>
       </c>
       <c r="B17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" t="s">
         <v>29</v>
-      </c>
-      <c r="D17" t="s">
-        <v>30</v>
       </c>
       <c r="H17" s="13">
         <v>0.1</v>
@@ -2457,18 +2457,18 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8">
         <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D18" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="H18" s="10">
         <v>0.1</v>
@@ -2478,18 +2478,18 @@
         <v>0.30000000000000004</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="8">
         <v>2</v>
       </c>
       <c r="B19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="D19" t="s">
         <v>33</v>
-      </c>
-      <c r="D19" t="s">
-        <v>34</v>
       </c>
       <c r="H19" s="13">
         <v>0.1</v>
@@ -2499,18 +2499,18 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="8">
         <v>1</v>
       </c>
       <c r="B20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="29" t="s">
+      <c r="D20" t="s">
         <v>36</v>
-      </c>
-      <c r="D20" t="s">
-        <v>37</v>
       </c>
       <c r="H20" s="13">
         <v>0.1</v>
@@ -2520,18 +2520,18 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="8">
         <v>1</v>
       </c>
       <c r="B21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="D21" t="s">
         <v>39</v>
-      </c>
-      <c r="D21" t="s">
-        <v>40</v>
       </c>
       <c r="H21" s="13">
         <v>0.1</v>
@@ -2541,18 +2541,18 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="8">
         <v>2</v>
       </c>
       <c r="B22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="29" t="s">
+      <c r="D22" t="s">
         <v>42</v>
-      </c>
-      <c r="D22" t="s">
-        <v>43</v>
       </c>
       <c r="H22" s="13">
         <v>0.1</v>
@@ -2562,18 +2562,18 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="8">
         <v>1</v>
       </c>
       <c r="B23" t="s">
+        <v>109</v>
+      </c>
+      <c r="C23" s="30" t="s">
         <v>110</v>
       </c>
-      <c r="C23" s="30" t="s">
+      <c r="D23" s="2" t="s">
         <v>111</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>112</v>
       </c>
       <c r="H23" s="13">
         <v>0.1</v>
@@ -2583,19 +2583,19 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="8">
         <v>1</v>
       </c>
       <c r="B24" t="s">
+        <v>130</v>
+      </c>
+      <c r="C24" s="32" t="s">
         <v>131</v>
-      </c>
-      <c r="C24" s="32" t="s">
-        <v>132</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H24" s="10">
         <v>0.39</v>
@@ -2605,21 +2605,21 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="8">
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D25" t="s">
         <v>20</v>
       </c>
       <c r="F25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H25" s="10">
         <v>31.5</v>
@@ -2629,21 +2629,21 @@
         <v>31.5</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="8">
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D26" t="s">
         <v>20</v>
       </c>
       <c r="F26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H26" s="10">
         <v>14.4</v>
@@ -2653,18 +2653,18 @@
         <v>14.4</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="8">
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C27" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" t="s">
         <v>47</v>
-      </c>
-      <c r="D27" t="s">
-        <v>48</v>
       </c>
       <c r="H27" s="13">
         <v>1.7</v>
@@ -2674,18 +2674,18 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="8">
         <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C28" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="D28" t="s">
         <v>49</v>
-      </c>
-      <c r="D28" t="s">
-        <v>50</v>
       </c>
       <c r="H28" s="13">
         <v>0.46</v>
@@ -2695,18 +2695,18 @@
         <v>0.46</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="8">
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C29" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D29" t="s">
         <v>51</v>
-      </c>
-      <c r="D29" t="s">
-        <v>52</v>
       </c>
       <c r="H29" s="13">
         <v>1.69</v>
@@ -2716,18 +2716,18 @@
         <v>1.69</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="8">
         <v>1</v>
       </c>
       <c r="B30" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="C30" s="29" t="s">
+      <c r="D30" t="s">
         <v>54</v>
-      </c>
-      <c r="D30" t="s">
-        <v>55</v>
       </c>
       <c r="H30" s="13">
         <v>1.66</v>
@@ -2737,18 +2737,18 @@
         <v>1.66</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="8">
         <v>1</v>
       </c>
       <c r="B31" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="D31" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H31" s="13">
         <v>5.0199999999999996</v>
@@ -2758,18 +2758,18 @@
         <v>5.0199999999999996</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="8">
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D32" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="H32" s="13">
         <v>1.71</v>
@@ -2779,18 +2779,18 @@
         <v>1.71</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="8">
         <v>1</v>
       </c>
       <c r="B33" t="s">
+        <v>89</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="E33" t="s">
         <v>91</v>
-      </c>
-      <c r="E33" t="s">
-        <v>92</v>
       </c>
       <c r="H33" s="10">
         <v>0.02</v>
@@ -2800,21 +2800,21 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="8">
         <v>1</v>
       </c>
       <c r="B34" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D34" t="s">
         <v>20</v>
       </c>
       <c r="E34" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H34" s="10">
         <v>0.22</v>
@@ -2824,21 +2824,21 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="8">
         <v>4</v>
       </c>
       <c r="B35" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D35" t="s">
         <v>20</v>
       </c>
       <c r="E35" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H35" s="10">
         <v>0.5</v>
@@ -2848,24 +2848,24 @@
         <v>0.5</v>
       </c>
       <c r="J35" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="8">
         <v>5</v>
       </c>
       <c r="B36" t="s">
+        <v>60</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="D36" t="s">
         <v>20</v>
       </c>
       <c r="E36" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H36" s="10">
         <v>0.14000000000000001</v>
@@ -2875,15 +2875,15 @@
         <v>0.70000000000000007</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="8">
         <v>1</v>
       </c>
       <c r="B37" t="s">
+        <v>63</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="D37" t="s">
         <v>20</v>
@@ -2892,7 +2892,7 @@
         <v>20</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H37" s="10">
         <v>0.48</v>
@@ -2902,15 +2902,15 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="8">
         <v>1</v>
       </c>
       <c r="B38" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D38" t="s">
         <v>20</v>
@@ -2919,7 +2919,7 @@
         <v>20</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H38" s="10">
         <v>0.48</v>
@@ -2929,21 +2929,21 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="8">
         <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E39" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G39" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H39" s="10">
         <v>0.13</v>
@@ -2953,18 +2953,18 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="8">
         <v>1</v>
       </c>
       <c r="B40" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G40" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H40" s="10">
         <v>0.8</v>
@@ -2974,21 +2974,21 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="8">
         <v>2</v>
       </c>
       <c r="B41" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D41" t="s">
         <v>20</v>
       </c>
       <c r="E41" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H41" s="10">
         <v>0.02</v>
@@ -2998,18 +2998,18 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="8">
         <v>2</v>
       </c>
       <c r="B42" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E42" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H42" s="10">
         <v>0.79</v>
@@ -3019,21 +3019,21 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="8">
         <v>1</v>
       </c>
       <c r="B43" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D43" t="s">
         <v>20</v>
       </c>
       <c r="E43" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H43" s="10">
         <v>0.02</v>
@@ -3043,18 +3043,18 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="8">
         <v>1</v>
       </c>
       <c r="B44" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E44" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="H44" s="10">
         <v>0.18</v>
@@ -3064,18 +3064,18 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="8">
         <v>1</v>
       </c>
       <c r="B45" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E45" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H45" s="10">
         <v>0.02</v>
@@ -3085,18 +3085,18 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="8">
         <v>1</v>
       </c>
       <c r="B46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E46" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H46" s="10">
         <v>0.17</v>
@@ -3106,18 +3106,18 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="8">
         <v>1</v>
       </c>
       <c r="B47" t="s">
+        <v>122</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C47" s="1" t="s">
-        <v>124</v>
-      </c>
       <c r="E47" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H47" s="10">
         <v>0.79</v>
@@ -3126,18 +3126,18 @@
         <v>0</v>
       </c>
       <c r="J47" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="8">
         <v>1</v>
       </c>
       <c r="B48" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E48" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H48" s="10">
         <v>0.5</v>
@@ -3147,15 +3147,15 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="8">
         <v>1</v>
       </c>
       <c r="B49" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E49" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H49" s="10">
         <v>0.22</v>
@@ -3165,18 +3165,18 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="8">
         <v>1</v>
       </c>
       <c r="B50" t="s">
+        <v>83</v>
+      </c>
+      <c r="C50" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C50" s="1" t="s">
-        <v>85</v>
-      </c>
       <c r="D50" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E50" t="s">
         <v>20</v>
@@ -3189,18 +3189,18 @@
         <v>9.35</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="8">
         <v>2</v>
       </c>
       <c r="B51" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D51" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H51" s="10">
         <v>0.87</v>
@@ -3210,36 +3210,36 @@
         <v>1.74</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="9">
         <v>1</v>
       </c>
       <c r="B52" t="s">
+        <v>128</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C52" s="1" t="s">
-        <v>130</v>
-      </c>
       <c r="I52" s="15"/>
     </row>
-    <row r="53" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="8">
         <f>SUM(A2:A52)</f>
         <v>104</v>
       </c>
       <c r="I53" s="14">
         <f>SUM(I2:I52)</f>
-        <v>93.749999999999986</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>96.529999999999987</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B54" s="7" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B56" s="17" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -3254,25 +3254,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{654AF2B0-A25E-4579-92A7-2605A258747F}">
   <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8" style="8" customWidth="1"/>
-    <col min="2" max="2" width="36.36328125" customWidth="1"/>
+    <col min="2" max="2" width="36.33203125" customWidth="1"/>
     <col min="3" max="3" width="61" customWidth="1"/>
-    <col min="4" max="4" width="26.54296875" customWidth="1"/>
+    <col min="4" max="4" width="26.5546875" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
-    <col min="6" max="6" width="16.26953125" customWidth="1"/>
-    <col min="7" max="7" width="14.81640625" customWidth="1"/>
-    <col min="8" max="8" width="11.36328125" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.21875" customWidth="1"/>
+    <col min="7" max="7" width="14.77734375" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -3289,22 +3289,22 @@
         <v>4</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
         <v>13</v>
       </c>
@@ -3312,7 +3312,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -3325,18 +3325,18 @@
         <v>0.70199999999999996</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" t="s">
         <v>73</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>74</v>
-      </c>
-      <c r="D3" t="s">
-        <v>75</v>
       </c>
       <c r="H3" s="13">
         <v>0.1</v>
@@ -3346,7 +3346,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <v>2</v>
       </c>
@@ -3354,10 +3354,10 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H4" s="13">
         <v>0.17</v>
@@ -3367,7 +3367,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>10</v>
       </c>
@@ -3375,10 +3375,10 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H5" s="10">
         <v>0.28999999999999998</v>
@@ -3388,7 +3388,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <v>3</v>
       </c>
@@ -3409,7 +3409,7 @@
         <v>1.17</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>3</v>
       </c>
@@ -3420,7 +3420,7 @@
         <v>18</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>20</v>
@@ -3433,7 +3433,7 @@
         <v>0.84000000000000008</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <v>4</v>
       </c>
@@ -3441,16 +3441,16 @@
         <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>20</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H8" s="13">
         <v>1.41</v>
@@ -3460,7 +3460,7 @@
         <v>5.64</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <v>3</v>
       </c>
@@ -3471,7 +3471,7 @@
         <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E9" t="s">
         <v>20</v>
@@ -3484,42 +3484,42 @@
         <v>1.41</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>141</v>
+        <v>175</v>
       </c>
       <c r="C10" t="s">
         <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>24</v>
+        <v>176</v>
       </c>
       <c r="E10" t="s">
         <v>20</v>
       </c>
       <c r="H10" s="13">
-        <v>2.27</v>
+        <v>5.05</v>
       </c>
       <c r="I10" s="14">
         <f t="shared" si="0"/>
-        <v>2.27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>5.05</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <v>3</v>
       </c>
       <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
         <v>25</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>26</v>
-      </c>
-      <c r="D11" t="s">
-        <v>27</v>
       </c>
       <c r="H11" s="13">
         <v>0.1</v>
@@ -3529,18 +3529,18 @@
         <v>0.30000000000000004</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8">
         <v>1</v>
       </c>
       <c r="B12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" t="s">
         <v>77</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>78</v>
-      </c>
-      <c r="D12" t="s">
-        <v>79</v>
       </c>
       <c r="H12" s="13">
         <v>0.1</v>
@@ -3550,18 +3550,18 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8">
         <v>2</v>
       </c>
       <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
         <v>28</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>29</v>
-      </c>
-      <c r="D13" t="s">
-        <v>30</v>
       </c>
       <c r="H13" s="13">
         <v>0.1</v>
@@ -3571,18 +3571,18 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8">
         <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D14" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="H14" s="10">
         <v>0.1</v>
@@ -3592,18 +3592,18 @@
         <v>0.30000000000000004</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8">
         <v>2</v>
       </c>
       <c r="B15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" t="s">
         <v>32</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>33</v>
-      </c>
-      <c r="D15" t="s">
-        <v>34</v>
       </c>
       <c r="H15" s="13">
         <v>0.1</v>
@@ -3613,18 +3613,18 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8">
         <v>1</v>
       </c>
       <c r="B16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" t="s">
         <v>38</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>39</v>
-      </c>
-      <c r="D16" t="s">
-        <v>40</v>
       </c>
       <c r="H16" s="13">
         <v>0.1</v>
@@ -3634,19 +3634,19 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8">
         <v>1</v>
       </c>
       <c r="B17" t="s">
+        <v>130</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>131</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>132</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H17" s="10">
         <v>0.39</v>
@@ -3656,21 +3656,21 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8">
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D18" t="s">
         <v>20</v>
       </c>
       <c r="F18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H18" s="10">
         <v>31.5</v>
@@ -3680,21 +3680,21 @@
         <v>31.5</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="8">
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D19" t="s">
         <v>20</v>
       </c>
       <c r="F19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H19" s="10">
         <v>14.4</v>
@@ -3704,18 +3704,18 @@
         <v>14.4</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="8">
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C20" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" t="s">
         <v>47</v>
-      </c>
-      <c r="D20" t="s">
-        <v>48</v>
       </c>
       <c r="H20" s="13">
         <v>1.7</v>
@@ -3725,18 +3725,18 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="8">
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C21" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" t="s">
         <v>51</v>
-      </c>
-      <c r="D21" t="s">
-        <v>52</v>
       </c>
       <c r="H21" s="13">
         <v>1.69</v>
@@ -3746,18 +3746,18 @@
         <v>1.69</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="8">
         <v>1</v>
       </c>
       <c r="B22" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" t="s">
         <v>56</v>
       </c>
-      <c r="C22" t="s">
-        <v>57</v>
-      </c>
       <c r="D22" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H22" s="13">
         <v>5.0199999999999996</v>
@@ -3767,18 +3767,18 @@
         <v>5.0199999999999996</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="8">
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D23" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="H23" s="13">
         <v>1.71</v>
@@ -3788,18 +3788,18 @@
         <v>1.71</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="8">
         <v>1</v>
       </c>
       <c r="B24" t="s">
+        <v>89</v>
+      </c>
+      <c r="C24" t="s">
         <v>90</v>
       </c>
-      <c r="C24" t="s">
+      <c r="E24" t="s">
         <v>91</v>
-      </c>
-      <c r="E24" t="s">
-        <v>92</v>
       </c>
       <c r="H24" s="10">
         <v>0.02</v>
@@ -3809,21 +3809,21 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="8">
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D25" t="s">
         <v>20</v>
       </c>
       <c r="E25" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H25" s="10">
         <v>0.22</v>
@@ -3833,21 +3833,21 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="8">
         <v>4</v>
       </c>
       <c r="B26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C26" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D26" t="s">
         <v>20</v>
       </c>
       <c r="E26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H26" s="10">
         <v>0.5</v>
@@ -3857,24 +3857,24 @@
         <v>0.5</v>
       </c>
       <c r="J26" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="8">
         <v>5</v>
       </c>
       <c r="B27" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" t="s">
         <v>61</v>
-      </c>
-      <c r="C27" t="s">
-        <v>62</v>
       </c>
       <c r="D27" t="s">
         <v>20</v>
       </c>
       <c r="E27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H27" s="10">
         <v>0.14000000000000001</v>
@@ -3884,15 +3884,15 @@
         <v>0.70000000000000007</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="8">
         <v>1</v>
       </c>
       <c r="B28" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" t="s">
         <v>64</v>
-      </c>
-      <c r="C28" t="s">
-        <v>65</v>
       </c>
       <c r="D28" t="s">
         <v>20</v>
@@ -3901,7 +3901,7 @@
         <v>20</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H28" s="10">
         <v>0.48</v>
@@ -3911,15 +3911,15 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="8">
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D29" t="s">
         <v>20</v>
@@ -3928,7 +3928,7 @@
         <v>20</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H29" s="10">
         <v>0.48</v>
@@ -3938,21 +3938,21 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="8">
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E30" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H30" s="10">
         <v>0.13</v>
@@ -3962,18 +3962,18 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="8">
         <v>1</v>
       </c>
       <c r="B31" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C31" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G31" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H31" s="10">
         <v>0.8</v>
@@ -3983,21 +3983,21 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="8">
         <v>2</v>
       </c>
       <c r="B32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C32" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D32" t="s">
         <v>20</v>
       </c>
       <c r="E32" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H32" s="10">
         <v>0.02</v>
@@ -4007,18 +4007,18 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="8">
         <v>2</v>
       </c>
       <c r="B33" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C33" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E33" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H33" s="10">
         <v>0.79</v>
@@ -4028,21 +4028,21 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="8">
         <v>1</v>
       </c>
       <c r="B34" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C34" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D34" t="s">
         <v>20</v>
       </c>
       <c r="E34" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H34" s="10">
         <v>0.02</v>
@@ -4052,18 +4052,18 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="8">
         <v>1</v>
       </c>
       <c r="B35" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C35" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E35" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="H35" s="10">
         <v>0.18</v>
@@ -4073,18 +4073,18 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="8">
         <v>1</v>
       </c>
       <c r="B36" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C36" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E36" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H36" s="10">
         <v>0.02</v>
@@ -4094,18 +4094,18 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="8">
         <v>1</v>
       </c>
       <c r="B37" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C37" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E37" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H37" s="10">
         <v>0.17</v>
@@ -4115,18 +4115,18 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="8">
         <v>1</v>
       </c>
       <c r="B38" t="s">
+        <v>122</v>
+      </c>
+      <c r="C38" t="s">
         <v>123</v>
       </c>
-      <c r="C38" t="s">
-        <v>124</v>
-      </c>
       <c r="E38" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H38" s="10">
         <v>0.79</v>
@@ -4135,18 +4135,18 @@
         <v>0</v>
       </c>
       <c r="J38" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="8">
         <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E39" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H39" s="10">
         <v>0.5</v>
@@ -4156,15 +4156,15 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="8">
         <v>1</v>
       </c>
       <c r="B40" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E40" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H40" s="10">
         <v>0.22</v>
@@ -4174,18 +4174,18 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="8">
         <v>1</v>
       </c>
       <c r="B41" t="s">
+        <v>83</v>
+      </c>
+      <c r="C41" t="s">
         <v>84</v>
       </c>
-      <c r="C41" t="s">
-        <v>85</v>
-      </c>
       <c r="D41" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E41" t="s">
         <v>20</v>
@@ -4198,18 +4198,18 @@
         <v>9.35</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="8">
         <v>2</v>
       </c>
       <c r="B42" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C42" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D42" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H42" s="10">
         <v>0.87</v>
@@ -4219,31 +4219,31 @@
         <v>1.74</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="9">
         <v>1</v>
       </c>
       <c r="B43" t="s">
+        <v>128</v>
+      </c>
+      <c r="C43" t="s">
         <v>129</v>
       </c>
-      <c r="C43" t="s">
-        <v>130</v>
-      </c>
       <c r="I43" s="15"/>
     </row>
-    <row r="44" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="8">
         <f>SUM(A2:A43)</f>
         <v>90</v>
       </c>
       <c r="I44" s="14">
         <f>SUM(I2:I43)</f>
-        <v>89.441999999999979</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>92.221999999999994</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -4259,17 +4259,17 @@
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8" style="8" customWidth="1"/>
-    <col min="2" max="2" width="36.36328125" customWidth="1"/>
+    <col min="2" max="2" width="36.33203125" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="26.54296875" customWidth="1"/>
-    <col min="5" max="5" width="11.36328125" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.5546875" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -4283,13 +4283,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
         <v>2</v>
       </c>
@@ -4297,7 +4297,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -4310,7 +4310,7 @@
         <v>0.108</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <v>1</v>
       </c>
@@ -4331,7 +4331,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <v>1</v>
       </c>
@@ -4339,10 +4339,10 @@
         <v>11</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E4" s="10">
         <v>0.28999999999999998</v>
@@ -4352,7 +4352,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>1</v>
       </c>
@@ -4363,7 +4363,7 @@
         <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E5" s="13">
         <v>0.24</v>
@@ -4373,18 +4373,18 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E6" s="13">
         <v>0.36</v>
@@ -4394,18 +4394,18 @@
         <v>0.72</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>1</v>
       </c>
       <c r="B7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="D7" t="s">
         <v>36</v>
-      </c>
-      <c r="D7" t="s">
-        <v>37</v>
       </c>
       <c r="E7" s="13">
         <v>0.1</v>
@@ -4415,18 +4415,18 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <v>2</v>
       </c>
       <c r="B8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="D8" t="s">
         <v>42</v>
-      </c>
-      <c r="D8" t="s">
-        <v>43</v>
       </c>
       <c r="E8" s="13">
         <v>0.1</v>
@@ -4436,18 +4436,18 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C9" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" t="s">
         <v>49</v>
-      </c>
-      <c r="D9" t="s">
-        <v>50</v>
       </c>
       <c r="E9" s="13">
         <v>0.46</v>
@@ -4457,18 +4457,18 @@
         <v>0.46</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
         <v>1</v>
       </c>
       <c r="B10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="D10" t="s">
         <v>54</v>
-      </c>
-      <c r="D10" t="s">
-        <v>55</v>
       </c>
       <c r="E10" s="13">
         <v>1.66</v>
@@ -4478,7 +4478,7 @@
         <v>1.66</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <f>SUM(A2:A10)</f>
         <v>12</v>
@@ -4488,14 +4488,14 @@
         <v>3.9279999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B13" s="17" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -4511,17 +4511,17 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8" style="8" customWidth="1"/>
-    <col min="2" max="2" width="36.36328125" customWidth="1"/>
+    <col min="2" max="2" width="36.33203125" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.54296875" customWidth="1"/>
-    <col min="5" max="5" width="11.36328125" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.5546875" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -4535,24 +4535,24 @@
         <v>3</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>109</v>
       </c>
       <c r="E2" s="13">
         <v>0.28000000000000003</v>
@@ -4562,18 +4562,18 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9">
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>111</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>112</v>
       </c>
       <c r="E3" s="13">
         <v>0.1</v>
@@ -4583,7 +4583,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <f>SUM(A2:A3)</f>
         <v>2</v>
@@ -4593,14 +4593,14 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B6" s="17" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>